<commit_message>
added question and changed video
</commit_message>
<xml_diff>
--- a/144F20/Topic 2/slope-intercept.xlsx
+++ b/144F20/Topic 2/slope-intercept.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\OneDrive - GCU Employees\Course Materials\git\Teaching\144F20\Topic 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="10_ncr:80_{57743E7C-1D0B-4E69-ACA8-2749DA19135A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E3EBC588-9FCB-4FB1-BFB7-BF123774F600}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="10_ncr:80_{57743E7C-1D0B-4E69-ACA8-2749DA19135A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C2BF989D-5849-4DAD-AEA9-D691A81325F5}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="20796" windowHeight="11424" xr2:uid="{DA857894-CCDD-4590-8F7E-A65A6A8D0808}"/>
+    <workbookView xWindow="1635" yWindow="1125" windowWidth="25995" windowHeight="14280" xr2:uid="{DA857894-CCDD-4590-8F7E-A65A6A8D0808}"/>
   </bookViews>
   <sheets>
     <sheet name="Linear Fit" sheetId="1" r:id="rId1"/>
@@ -184,7 +184,7 @@
     <t>Video for this.</t>
   </si>
   <si>
-    <t>See video above.</t>
+    <t xml:space="preserve">- Use your graph to approximate Y at X = 18:   Y = </t>
   </si>
 </sst>
 </file>
@@ -227,15 +227,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="14"/>
-      <color theme="10"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Comic Sans MS"/>
       <family val="4"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Comic Sans MS"/>
       <family val="4"/>
     </font>
@@ -569,7 +570,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -660,6 +661,9 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -698,12 +702,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -763,11 +761,26 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -785,6 +798,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE5CEACF-71AE-4AA4-9E21-BE8740C364A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2733675" y="19050"/>
+          <a:ext cx="352425" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1084,42 +1152,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28FDA598-8F75-47DB-A1EB-542124AF2F6A}">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
     <col min="8" max="8" width="4" customWidth="1"/>
-    <col min="9" max="10" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1">
-      <c r="C1" s="44" t="s">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1">
+      <c r="C1" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-    </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1">
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="I2" s="46" t="s">
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" thickBot="1">
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="I2" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="47"/>
-    </row>
-    <row r="3" spans="1:17" ht="16.2" thickBot="1">
-      <c r="B3" s="49" t="s">
+      <c r="J2" s="46"/>
+    </row>
+    <row r="3" spans="1:17" ht="17.25" thickBot="1">
+      <c r="B3" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="50"/>
       <c r="F3" s="30" t="s">
         <v>40</v>
       </c>
@@ -1138,7 +1207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15" thickBot="1">
+    <row r="5" spans="1:17" ht="15.75" thickBot="1">
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1152,11 +1221,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" thickBot="1">
-      <c r="A6" s="48" t="s">
+    <row r="6" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A6" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="48"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="24">
         <v>2</v>
       </c>
@@ -1171,7 +1240,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15" thickBot="1">
+    <row r="7" spans="1:17" ht="15.75" thickBot="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="25">
@@ -1192,7 +1261,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" thickBot="1">
+    <row r="8" spans="1:17" ht="15.75" thickBot="1">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="25">
@@ -1217,24 +1286,22 @@
         <f>IF(F$3="a word","Fill F3",SIGN(Random!B$20-Random!B$21)*5*'Linear Fit'!C9+6+SIGN(Random!B14-Random!B21)*Random!D15*10)</f>
         <v>Fill F3</v>
       </c>
-      <c r="F9" s="52" t="s">
+      <c r="F9" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="52"/>
-      <c r="J9" s="35" t="s">
+      <c r="G9" s="51"/>
+      <c r="J9" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="64" t="s">
-        <v>47</v>
-      </c>
-      <c r="P9" s="65"/>
-      <c r="Q9" s="65"/>
-    </row>
-    <row r="10" spans="1:17" ht="15" thickBot="1">
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="68"/>
+      <c r="P9" s="69"/>
+      <c r="Q9" s="69"/>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" thickBot="1">
       <c r="C10" s="25">
         <v>10</v>
       </c>
@@ -1242,15 +1309,15 @@
         <f>IF(F$3="a word","Fill F3",SIGN(Random!B$20-Random!B$21)*5*'Linear Fit'!C10+6+SIGN(Random!B15-Random!B22)*Random!D16*10)</f>
         <v>Fill F3</v>
       </c>
-      <c r="F10" s="62"/>
-      <c r="G10" s="63"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="40"/>
-    </row>
-    <row r="11" spans="1:17" ht="15" thickBot="1">
+      <c r="F10" s="61"/>
+      <c r="G10" s="62"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="41"/>
+    </row>
+    <row r="11" spans="1:17" ht="15.75" thickBot="1">
       <c r="C11" s="26">
         <v>12</v>
       </c>
@@ -1258,98 +1325,111 @@
         <f>IF(F$3="a word","Fill F3",SIGN(Random!B$20-Random!B$21)*5*'Linear Fit'!C11+6+SIGN(Random!B16-Random!B23)*Random!D17*10)</f>
         <v>Fill F3</v>
       </c>
-      <c r="J11" s="41"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="43"/>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="F12" s="53" t="s">
+      <c r="J11" s="42"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="44"/>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" thickBot="1">
+      <c r="F12" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="54"/>
-      <c r="H12" s="55"/>
-    </row>
-    <row r="13" spans="1:17" ht="15" thickBot="1">
-      <c r="A13" s="52" t="s">
+      <c r="G12" s="53"/>
+      <c r="H12" s="54"/>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A13" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="52"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="56"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="58"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="57"/>
+      <c r="J13" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="64"/>
+      <c r="N13" s="65"/>
+      <c r="O13" s="67"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="51"/>
     </row>
     <row r="14" spans="1:17">
       <c r="C14" s="15">
         <v>-5</v>
       </c>
       <c r="D14" s="19"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="58"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="57"/>
     </row>
     <row r="15" spans="1:17">
       <c r="C15" s="16">
         <v>-3</v>
       </c>
       <c r="D15" s="20"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="58"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="57"/>
     </row>
     <row r="16" spans="1:17">
       <c r="C16" s="16">
         <v>0</v>
       </c>
       <c r="D16" s="20"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="58"/>
-    </row>
-    <row r="17" spans="3:8">
+      <c r="F16" s="55"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="57"/>
+    </row>
+    <row r="17" spans="3:13">
       <c r="C17" s="16">
         <v>7</v>
       </c>
       <c r="D17" s="20"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="58"/>
-    </row>
-    <row r="18" spans="3:8">
+      <c r="F17" s="55"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="57"/>
+    </row>
+    <row r="18" spans="3:13">
       <c r="C18" s="16">
         <v>13</v>
       </c>
       <c r="D18" s="20"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="58"/>
-    </row>
-    <row r="19" spans="3:8" ht="15" thickBot="1">
+      <c r="F18" s="55"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="57"/>
+    </row>
+    <row r="19" spans="3:13" ht="15.75" thickBot="1">
       <c r="C19" s="17">
         <v>20</v>
       </c>
       <c r="D19" s="21"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="61"/>
-    </row>
-    <row r="20" spans="3:8">
-      <c r="C20" s="31" t="s">
+      <c r="F19" s="58"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="60"/>
+    </row>
+    <row r="20" spans="3:13">
+      <c r="C20" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="32"/>
+      <c r="D20" s="33"/>
       <c r="F20" s="18"/>
     </row>
-    <row r="21" spans="3:8" ht="15" thickBot="1">
-      <c r="C21" s="33"/>
-      <c r="D21" s="34"/>
+    <row r="21" spans="3:13" ht="15.75" thickBot="1">
+      <c r="C21" s="34"/>
+      <c r="D21" s="35"/>
+    </row>
+    <row r="24" spans="3:13">
+      <c r="M24" s="31"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0"/>
@@ -1360,24 +1440,26 @@
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
   </customSheetViews>
-  <mergeCells count="11">
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="C20:D21"/>
-    <mergeCell ref="J9:N11"/>
-    <mergeCell ref="C1:E2"/>
-    <mergeCell ref="I2:J2"/>
+  <mergeCells count="12">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="F12:H19"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="F10:G10"/>
+    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="J9:N11"/>
+    <mergeCell ref="C1:E2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="O13:Q13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C1:E2" r:id="rId2" display="Video for this." xr:uid="{034F62B5-D6DE-4BF0-9A4B-D4FBF4CED3BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1389,7 +1471,7 @@
       <selection activeCell="B6" sqref="B6:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="H1">

</xml_diff>